<commit_message>
a traves de vscode
</commit_message>
<xml_diff>
--- a/excel files/equipos.xlsx
+++ b/excel files/equipos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\quemar\Programacion\app ntt backup\app backup + pyats + fmc\excel files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\quemar\Programacion\app ntt backup\app backup + pyats + fmc v1.1\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>hostname</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>alex</t>
+  </si>
+  <si>
+    <t>NXOS</t>
+  </si>
+  <si>
+    <t>192.168.0.212</t>
+  </si>
+  <si>
+    <t>nx</t>
   </si>
 </sst>
 </file>
@@ -464,7 +473,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,14 +542,30 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>

</xml_diff>